<commit_message>
Add source metadata documentation
</commit_message>
<xml_diff>
--- a/standards/cstdefinexml21/source/standards/doc/source_metadata_structure.xlsx
+++ b/standards/cstdefinexml21/source/standards/doc/source_metadata_structure.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="258">
   <si>
     <t>Obs</t>
   </si>
@@ -253,7 +253,7 @@
     <t>Observation Class within Standard</t>
   </si>
   <si>
-    <t>NCIt: C103329</t>
+    <t>NCIt: C103329 - [ADAM OTHER, C103375 BASIC DATA STRUCTURE, DEVICE LEVEL ANALYSIS DATASET, EVENTS, FINDINGS, FINDINGS ABOUT, INTERVENTIONS, MEDICAL DEVICE BASIC DATA STRUCTURE, MEDICAL DEVICE OCCURRENCE DATA STRUCTURE, OCCURRENCE DATA STRUCTURE, RELATIONSHIP, SPECIAL PURPOSE, STUDY REFERENCE, SUBJECT LEVEL ANALYSIS DATASET, TRIAL DESIGN]</t>
   </si>
   <si>
     <t>subclass</t>
@@ -262,7 +262,7 @@
     <t>Observation SubClass within Standard</t>
   </si>
   <si>
-    <t>NCIt: C165635, C177903, C176227,</t>
+    <t>NCIt: C165635, C177903, C176227 - [ADVERSE EVENT, MEDICAL DEVICE TIME-TO-EVENT, NON-COMPARTMENTAL ANALYSIS, POPULATION PHARMACOKINETIC ANALYSIS, TIME-TO-EVENT]</t>
   </si>
   <si>
     <t>xmlpath</t>
@@ -313,9 +313,6 @@
     <t>Release Date</t>
   </si>
   <si>
-    <t>NCIt: C170452 - [ADaMIG, BIMO, CDISC/NCI, SDTMIG, SDTMIG-AP, SDTMIG-MD, SENDIG, SENDIG-AR, SENDIG-DART</t>
-  </si>
-  <si>
     <t>isnonstandard</t>
   </si>
   <si>
@@ -409,7 +406,7 @@
     <t>Column Origin Type</t>
   </si>
   <si>
-    <t>NCIt: C170449 - [Assigned, Collect, Derived, Not Available, Other, Predecessor, Protocol]</t>
+    <t>NCIt: C170449 - [Assigned, Collected, Derived, Not Available, Other, Predecessor, Protocol]</t>
   </si>
   <si>
     <t>originsource</t>
@@ -616,7 +613,7 @@
     <t>Name of the external codelist</t>
   </si>
   <si>
-    <t>NCTt: C66788</t>
+    <t>NCTt: C66788 - [CDISC CT, COSTART, CTCAE, D-U-N-S NUMBER, ICD, ICD-O, LOINC, MED-RT, MedDRA, SNOMED, UNII, WHO ATC CLASSIFICATION SYSTEM, WHOART, WHODD]</t>
   </si>
   <si>
     <t>version</t>
@@ -1046,7 +1043,7 @@
     <col min="6" max="6" width="42.71" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.71" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.71" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="53.71" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="88.71" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="29" customHeight="1">
@@ -2035,7 +2032,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" ht="43" customHeight="1">
+    <row r="35" ht="87" customHeight="1">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2351,7 +2348,7 @@
         <v>40</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" ht="43" customHeight="1">
@@ -2397,10 +2394,10 @@
         <v>21</v>
       </c>
       <c r="E47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>13</v>
@@ -2409,7 +2406,7 @@
         <v>3</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" ht="43" customHeight="1">
@@ -2426,10 +2423,10 @@
         <v>22</v>
       </c>
       <c r="E48" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>13</v>
@@ -2438,7 +2435,7 @@
         <v>3</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" ht="43" customHeight="1">
@@ -2533,10 +2530,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D52" s="4">
         <v>1</v>
@@ -2562,10 +2559,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D53" s="4">
         <v>2</v>
@@ -2591,19 +2588,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D54" s="4">
         <v>3</v>
       </c>
       <c r="E54" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>13</v>
@@ -2620,10 +2617,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D55" s="4">
         <v>4</v>
@@ -2632,7 +2629,7 @@
         <v>64</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>13</v>
@@ -2649,10 +2646,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D56" s="4">
         <v>5</v>
@@ -2661,7 +2658,7 @@
         <v>47</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>49</v>
@@ -2678,10 +2675,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D57" s="4">
         <v>6</v>
@@ -2690,7 +2687,7 @@
         <v>50</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>13</v>
@@ -2699,7 +2696,7 @@
         <v>1</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" ht="43" customHeight="1">
@@ -2707,19 +2704,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D58" s="4">
         <v>7</v>
       </c>
       <c r="E58" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F58" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>49</v>
@@ -2736,19 +2733,19 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D59" s="4">
         <v>8</v>
       </c>
       <c r="E59" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F59" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>13</v>
@@ -2765,19 +2762,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D60" s="4">
         <v>9</v>
       </c>
       <c r="E60" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F60" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>49</v>
@@ -2794,19 +2791,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D61" s="4">
         <v>10</v>
       </c>
       <c r="E61" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>13</v>
@@ -2815,7 +2812,7 @@
         <v>18</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" ht="43" customHeight="1">
@@ -2823,19 +2820,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D62" s="4">
         <v>11</v>
       </c>
       <c r="E62" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>13</v>
@@ -2852,19 +2849,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D63" s="4">
         <v>12</v>
       </c>
       <c r="E63" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>124</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>13</v>
@@ -2873,7 +2870,7 @@
         <v>10</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" ht="43" customHeight="1">
@@ -2881,19 +2878,19 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="D64" s="4">
         <v>13</v>
       </c>
       <c r="E64" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>13</v>
@@ -2910,19 +2907,19 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="D65" s="4">
         <v>14</v>
       </c>
       <c r="E65" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F65" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>13</v>
@@ -2931,7 +2928,7 @@
         <v>40</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" ht="43" customHeight="1">
@@ -2939,19 +2936,19 @@
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D66" s="4">
         <v>15</v>
       </c>
       <c r="E66" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>13</v>
@@ -2960,7 +2957,7 @@
         <v>40</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="67" ht="43" customHeight="1">
@@ -2968,19 +2965,19 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D67" s="4">
         <v>16</v>
       </c>
       <c r="E67" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>13</v>
@@ -2997,19 +2994,19 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D68" s="4">
         <v>17</v>
       </c>
       <c r="E68" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F68" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>13</v>
@@ -3026,19 +3023,19 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D69" s="4">
         <v>18</v>
       </c>
       <c r="E69" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>13</v>
@@ -3055,19 +3052,19 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D70" s="4">
         <v>19</v>
       </c>
       <c r="E70" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>13</v>
@@ -3084,19 +3081,19 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D71" s="4">
         <v>20</v>
       </c>
       <c r="E71" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F71" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>13</v>
@@ -3105,7 +3102,7 @@
         <v>11</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="72" ht="43" customHeight="1">
@@ -3113,19 +3110,19 @@
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C72" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D72" s="4">
         <v>21</v>
       </c>
       <c r="E72" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F72" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>13</v>
@@ -3142,19 +3139,19 @@
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D73" s="4">
         <v>22</v>
       </c>
       <c r="E73" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F73" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>13</v>
@@ -3171,10 +3168,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D74" s="4">
         <v>23</v>
@@ -3200,19 +3197,19 @@
         <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D75" s="4">
         <v>24</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>13</v>
@@ -3221,7 +3218,7 @@
         <v>3</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="76" ht="43" customHeight="1">
@@ -3229,19 +3226,19 @@
         <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D76" s="4">
         <v>25</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>13</v>
@@ -3250,7 +3247,7 @@
         <v>3</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="77" ht="43" customHeight="1">
@@ -3258,10 +3255,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C77" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D77" s="4">
         <v>26</v>
@@ -3287,10 +3284,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D78" s="4">
         <v>27</v>
@@ -3316,10 +3313,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C79" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="D79" s="4">
         <v>28</v>
@@ -3345,10 +3342,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D80" s="4">
         <v>1</v>
@@ -3374,10 +3371,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D81" s="4">
         <v>2</v>
@@ -3403,19 +3400,19 @@
         <v>81</v>
       </c>
       <c r="B82" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C82" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D82" s="4">
         <v>3</v>
       </c>
       <c r="E82" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F82" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="G82" s="5" t="s">
         <v>13</v>
@@ -3432,19 +3429,19 @@
         <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D83" s="4">
         <v>4</v>
       </c>
       <c r="E83" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F83" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="F83" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="G83" s="5" t="s">
         <v>13</v>
@@ -3461,19 +3458,19 @@
         <v>83</v>
       </c>
       <c r="B84" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C84" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D84" s="4">
         <v>5</v>
       </c>
       <c r="E84" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F84" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="F84" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="G84" s="5" t="s">
         <v>13</v>
@@ -3490,19 +3487,19 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D85" s="4">
         <v>6</v>
       </c>
       <c r="E85" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F85" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="G85" s="5" t="s">
         <v>13</v>
@@ -3519,19 +3516,19 @@
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D86" s="4">
         <v>7</v>
       </c>
       <c r="E86" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F86" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="G86" s="5" t="s">
         <v>13</v>
@@ -3548,10 +3545,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C87" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D87" s="4">
         <v>8</v>
@@ -3560,7 +3557,7 @@
         <v>64</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G87" s="5" t="s">
         <v>13</v>
@@ -3577,10 +3574,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D88" s="4">
         <v>9</v>
@@ -3589,7 +3586,7 @@
         <v>47</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G88" s="5" t="s">
         <v>49</v>
@@ -3606,10 +3603,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C89" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D89" s="4">
         <v>10</v>
@@ -3618,7 +3615,7 @@
         <v>50</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G89" s="5" t="s">
         <v>13</v>
@@ -3627,7 +3624,7 @@
         <v>1</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="90" ht="43" customHeight="1">
@@ -3635,19 +3632,19 @@
         <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C90" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D90" s="4">
         <v>11</v>
       </c>
       <c r="E90" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F90" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="G90" s="5" t="s">
         <v>49</v>
@@ -3664,19 +3661,19 @@
         <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D91" s="4">
         <v>12</v>
       </c>
       <c r="E91" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F91" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="G91" s="5" t="s">
         <v>13</v>
@@ -3693,19 +3690,19 @@
         <v>91</v>
       </c>
       <c r="B92" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C92" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C92" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="D92" s="4">
         <v>13</v>
       </c>
       <c r="E92" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F92" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="G92" s="5" t="s">
         <v>49</v>
@@ -3722,19 +3719,19 @@
         <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C93" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C93" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="D93" s="4">
         <v>14</v>
       </c>
       <c r="E93" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F93" s="3" t="s">
         <v>118</v>
-      </c>
-      <c r="F93" s="3" t="s">
-        <v>119</v>
       </c>
       <c r="G93" s="5" t="s">
         <v>13</v>
@@ -3743,7 +3740,7 @@
         <v>18</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="94" ht="43" customHeight="1">
@@ -3751,19 +3748,19 @@
         <v>93</v>
       </c>
       <c r="B94" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C94" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D94" s="4">
         <v>15</v>
       </c>
       <c r="E94" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F94" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>13</v>
@@ -3780,19 +3777,19 @@
         <v>94</v>
       </c>
       <c r="B95" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C95" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C95" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D95" s="4">
         <v>16</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G95" s="5" t="s">
         <v>13</v>
@@ -3801,7 +3798,7 @@
         <v>10</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="96" ht="43" customHeight="1">
@@ -3809,19 +3806,19 @@
         <v>95</v>
       </c>
       <c r="B96" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C96" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D96" s="4">
         <v>17</v>
       </c>
       <c r="E96" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F96" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="G96" s="5" t="s">
         <v>13</v>
@@ -3838,19 +3835,19 @@
         <v>96</v>
       </c>
       <c r="B97" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C97" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D97" s="4">
         <v>18</v>
       </c>
       <c r="E97" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F97" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="G97" s="5" t="s">
         <v>13</v>
@@ -3859,7 +3856,7 @@
         <v>40</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="98" ht="43" customHeight="1">
@@ -3867,19 +3864,19 @@
         <v>97</v>
       </c>
       <c r="B98" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C98" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D98" s="4">
         <v>19</v>
       </c>
       <c r="E98" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F98" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="G98" s="5" t="s">
         <v>13</v>
@@ -3888,7 +3885,7 @@
         <v>40</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="99" ht="43" customHeight="1">
@@ -3896,19 +3893,19 @@
         <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D99" s="4">
         <v>20</v>
       </c>
       <c r="E99" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F99" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="G99" s="5" t="s">
         <v>13</v>
@@ -3925,19 +3922,19 @@
         <v>99</v>
       </c>
       <c r="B100" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C100" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D100" s="4">
         <v>21</v>
       </c>
       <c r="E100" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F100" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="G100" s="5" t="s">
         <v>13</v>
@@ -3954,19 +3951,19 @@
         <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C101" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D101" s="4">
         <v>22</v>
       </c>
       <c r="E101" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F101" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="G101" s="5" t="s">
         <v>13</v>
@@ -3983,19 +3980,19 @@
         <v>101</v>
       </c>
       <c r="B102" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C102" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D102" s="4">
         <v>23</v>
       </c>
       <c r="E102" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F102" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="F102" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="G102" s="5" t="s">
         <v>13</v>
@@ -4012,19 +4009,19 @@
         <v>102</v>
       </c>
       <c r="B103" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C103" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C103" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D103" s="4">
         <v>24</v>
       </c>
       <c r="E103" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F103" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>143</v>
       </c>
       <c r="G103" s="5" t="s">
         <v>13</v>
@@ -4033,7 +4030,7 @@
         <v>11</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="104" ht="43" customHeight="1">
@@ -4041,19 +4038,19 @@
         <v>103</v>
       </c>
       <c r="B104" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C104" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D104" s="4">
         <v>25</v>
       </c>
       <c r="E104" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F104" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="G104" s="5" t="s">
         <v>13</v>
@@ -4070,19 +4067,19 @@
         <v>104</v>
       </c>
       <c r="B105" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C105" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C105" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D105" s="4">
         <v>26</v>
       </c>
       <c r="E105" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F105" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="G105" s="5" t="s">
         <v>13</v>
@@ -4099,10 +4096,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C106" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D106" s="4">
         <v>27</v>
@@ -4128,19 +4125,19 @@
         <v>106</v>
       </c>
       <c r="B107" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D107" s="4">
         <v>28</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G107" s="5" t="s">
         <v>13</v>
@@ -4149,7 +4146,7 @@
         <v>3</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" ht="43" customHeight="1">
@@ -4157,10 +4154,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C108" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D108" s="4">
         <v>29</v>
@@ -4186,10 +4183,10 @@
         <v>108</v>
       </c>
       <c r="B109" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C109" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C109" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D109" s="4">
         <v>30</v>
@@ -4215,10 +4212,10 @@
         <v>109</v>
       </c>
       <c r="B110" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C110" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="C110" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="D110" s="4">
         <v>31</v>
@@ -4244,10 +4241,10 @@
         <v>110</v>
       </c>
       <c r="B111" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C111" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D111" s="4">
         <v>1</v>
@@ -4273,19 +4270,19 @@
         <v>111</v>
       </c>
       <c r="B112" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C112" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C112" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D112" s="4">
         <v>2</v>
       </c>
       <c r="E112" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F112" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>165</v>
       </c>
       <c r="G112" s="5" t="s">
         <v>13</v>
@@ -4302,19 +4299,19 @@
         <v>112</v>
       </c>
       <c r="B113" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C113" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C113" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D113" s="4">
         <v>3</v>
       </c>
       <c r="E113" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F113" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>167</v>
       </c>
       <c r="G113" s="5" t="s">
         <v>13</v>
@@ -4331,19 +4328,19 @@
         <v>113</v>
       </c>
       <c r="B114" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C114" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C114" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D114" s="4">
         <v>4</v>
       </c>
       <c r="E114" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F114" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="F114" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="G114" s="5" t="s">
         <v>13</v>
@@ -4360,19 +4357,19 @@
         <v>114</v>
       </c>
       <c r="B115" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C115" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D115" s="4">
         <v>5</v>
       </c>
       <c r="E115" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F115" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="F115" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="G115" s="5" t="s">
         <v>13</v>
@@ -4389,19 +4386,19 @@
         <v>115</v>
       </c>
       <c r="B116" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C116" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C116" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D116" s="4">
         <v>6</v>
       </c>
       <c r="E116" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F116" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="F116" s="3" t="s">
-        <v>173</v>
       </c>
       <c r="G116" s="5" t="s">
         <v>13</v>
@@ -4418,19 +4415,19 @@
         <v>116</v>
       </c>
       <c r="B117" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C117" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C117" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D117" s="4">
         <v>7</v>
       </c>
       <c r="E117" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F117" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="F117" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="G117" s="5" t="s">
         <v>13</v>
@@ -4439,7 +4436,7 @@
         <v>7</v>
       </c>
       <c r="I117" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="118" ht="43" customHeight="1">
@@ -4447,19 +4444,19 @@
         <v>117</v>
       </c>
       <c r="B118" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C118" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C118" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D118" s="4">
         <v>8</v>
       </c>
       <c r="E118" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F118" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="F118" s="3" t="s">
-        <v>178</v>
       </c>
       <c r="G118" s="5" t="s">
         <v>13</v>
@@ -4476,19 +4473,19 @@
         <v>118</v>
       </c>
       <c r="B119" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C119" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C119" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D119" s="4">
         <v>9</v>
       </c>
       <c r="E119" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="F119" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="F119" s="3" t="s">
-        <v>180</v>
       </c>
       <c r="G119" s="5" t="s">
         <v>13</v>
@@ -4505,19 +4502,19 @@
         <v>119</v>
       </c>
       <c r="B120" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C120" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C120" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D120" s="4">
         <v>10</v>
       </c>
       <c r="E120" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="F120" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="F120" s="3" t="s">
-        <v>182</v>
       </c>
       <c r="G120" s="5" t="s">
         <v>49</v>
@@ -4534,19 +4531,19 @@
         <v>120</v>
       </c>
       <c r="B121" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C121" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C121" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D121" s="4">
         <v>11</v>
       </c>
       <c r="E121" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F121" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="F121" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="G121" s="5" t="s">
         <v>13</v>
@@ -4563,19 +4560,19 @@
         <v>121</v>
       </c>
       <c r="B122" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C122" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C122" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D122" s="4">
         <v>12</v>
       </c>
       <c r="E122" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F122" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="F122" s="3" t="s">
-        <v>186</v>
       </c>
       <c r="G122" s="5" t="s">
         <v>13</v>
@@ -4592,19 +4589,19 @@
         <v>122</v>
       </c>
       <c r="B123" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C123" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C123" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="D123" s="4">
         <v>13</v>
       </c>
       <c r="E123" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F123" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="F123" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="G123" s="5" t="s">
         <v>13</v>
@@ -4621,19 +4618,19 @@
         <v>123</v>
       </c>
       <c r="B124" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C124" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="C124" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="D124" s="4">
         <v>14</v>
       </c>
       <c r="E124" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F124" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="F124" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="G124" s="5" t="s">
         <v>13</v>
@@ -4650,19 +4647,19 @@
         <v>124</v>
       </c>
       <c r="B125" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C125" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C125" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D125" s="4">
         <v>15</v>
       </c>
       <c r="E125" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F125" s="3" t="s">
         <v>191</v>
-      </c>
-      <c r="F125" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="G125" s="5" t="s">
         <v>49</v>
@@ -4679,19 +4676,19 @@
         <v>125</v>
       </c>
       <c r="B126" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C126" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C126" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D126" s="4">
         <v>16</v>
       </c>
       <c r="E126" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F126" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="F126" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="G126" s="5" t="s">
         <v>49</v>
@@ -4708,19 +4705,19 @@
         <v>126</v>
       </c>
       <c r="B127" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C127" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D127" s="4">
         <v>17</v>
       </c>
       <c r="E127" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="F127" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="F127" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="G127" s="5" t="s">
         <v>13</v>
@@ -4729,7 +4726,7 @@
         <v>3</v>
       </c>
       <c r="I127" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="128" ht="43" customHeight="1">
@@ -4737,19 +4734,19 @@
         <v>127</v>
       </c>
       <c r="B128" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C128" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D128" s="4">
         <v>18</v>
       </c>
       <c r="E128" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F128" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="F128" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="G128" s="5" t="s">
         <v>13</v>
@@ -4758,7 +4755,7 @@
         <v>200</v>
       </c>
       <c r="I128" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="129" ht="43" customHeight="1">
@@ -4766,19 +4763,19 @@
         <v>128</v>
       </c>
       <c r="B129" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C129" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D129" s="4">
         <v>19</v>
       </c>
       <c r="E129" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="F129" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="F129" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="G129" s="5" t="s">
         <v>13</v>
@@ -4795,19 +4792,19 @@
         <v>129</v>
       </c>
       <c r="B130" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C130" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D130" s="4">
         <v>20</v>
       </c>
       <c r="E130" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F130" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="F130" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="G130" s="5" t="s">
         <v>13</v>
@@ -4824,19 +4821,19 @@
         <v>130</v>
       </c>
       <c r="B131" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C131" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D131" s="4">
         <v>21</v>
       </c>
       <c r="E131" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F131" s="3" t="s">
         <v>204</v>
-      </c>
-      <c r="F131" s="3" t="s">
-        <v>205</v>
       </c>
       <c r="G131" s="5" t="s">
         <v>13</v>
@@ -4853,10 +4850,10 @@
         <v>131</v>
       </c>
       <c r="B132" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C132" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D132" s="4">
         <v>22</v>
@@ -4882,10 +4879,10 @@
         <v>132</v>
       </c>
       <c r="B133" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C133" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D133" s="4">
         <v>23</v>
@@ -4911,10 +4908,10 @@
         <v>133</v>
       </c>
       <c r="B134" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C134" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D134" s="4">
         <v>24</v>
@@ -4940,10 +4937,10 @@
         <v>134</v>
       </c>
       <c r="B135" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C135" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C135" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D135" s="4">
         <v>25</v>
@@ -4969,19 +4966,19 @@
         <v>135</v>
       </c>
       <c r="B136" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C136" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C136" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D136" s="4">
         <v>26</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G136" s="5" t="s">
         <v>13</v>
@@ -4990,7 +4987,7 @@
         <v>3</v>
       </c>
       <c r="I136" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="137" ht="43" customHeight="1">
@@ -4998,10 +4995,10 @@
         <v>136</v>
       </c>
       <c r="B137" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C137" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C137" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D137" s="4">
         <v>27</v>
@@ -5027,10 +5024,10 @@
         <v>137</v>
       </c>
       <c r="B138" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C138" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C138" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D138" s="4">
         <v>28</v>
@@ -5056,10 +5053,10 @@
         <v>138</v>
       </c>
       <c r="B139" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C139" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="D139" s="4">
         <v>29</v>
@@ -5085,10 +5082,10 @@
         <v>139</v>
       </c>
       <c r="B140" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C140" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D140" s="4">
         <v>1</v>
@@ -5114,19 +5111,19 @@
         <v>140</v>
       </c>
       <c r="B141" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C141" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C141" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D141" s="4">
         <v>2</v>
       </c>
       <c r="E141" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F141" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="F141" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="G141" s="5" t="s">
         <v>13</v>
@@ -5135,7 +5132,7 @@
         <v>32</v>
       </c>
       <c r="I141" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="142" ht="58" customHeight="1">
@@ -5143,19 +5140,19 @@
         <v>141</v>
       </c>
       <c r="B142" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C142" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D142" s="4">
         <v>3</v>
       </c>
       <c r="E142" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="F142" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="F142" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="G142" s="5" t="s">
         <v>13</v>
@@ -5164,7 +5161,7 @@
         <v>32</v>
       </c>
       <c r="I142" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="143" ht="43" customHeight="1">
@@ -5172,19 +5169,19 @@
         <v>142</v>
       </c>
       <c r="B143" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C143" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D143" s="4">
         <v>4</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G143" s="5" t="s">
         <v>13</v>
@@ -5201,19 +5198,19 @@
         <v>143</v>
       </c>
       <c r="B144" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C144" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D144" s="4">
         <v>5</v>
       </c>
       <c r="E144" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="F144" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="F144" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="G144" s="5" t="s">
         <v>13</v>
@@ -5230,19 +5227,19 @@
         <v>144</v>
       </c>
       <c r="B145" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C145" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D145" s="4">
         <v>6</v>
       </c>
       <c r="E145" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F145" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="F145" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="G145" s="5" t="s">
         <v>13</v>
@@ -5251,7 +5248,7 @@
         <v>32</v>
       </c>
       <c r="I145" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="146" ht="43" customHeight="1">
@@ -5259,19 +5256,19 @@
         <v>145</v>
       </c>
       <c r="B146" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C146" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C146" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D146" s="4">
         <v>7</v>
       </c>
       <c r="E146" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F146" s="3" t="s">
         <v>221</v>
-      </c>
-      <c r="F146" s="3" t="s">
-        <v>222</v>
       </c>
       <c r="G146" s="5" t="s">
         <v>13</v>
@@ -5288,19 +5285,19 @@
         <v>146</v>
       </c>
       <c r="B147" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C147" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D147" s="4">
         <v>8</v>
       </c>
       <c r="E147" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="F147" s="3" t="s">
         <v>223</v>
-      </c>
-      <c r="F147" s="3" t="s">
-        <v>224</v>
       </c>
       <c r="G147" s="5" t="s">
         <v>13</v>
@@ -5317,10 +5314,10 @@
         <v>147</v>
       </c>
       <c r="B148" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C148" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D148" s="4">
         <v>9</v>
@@ -5346,19 +5343,19 @@
         <v>148</v>
       </c>
       <c r="B149" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C149" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C149" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D149" s="4">
         <v>10</v>
       </c>
       <c r="E149" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F149" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="F149" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="G149" s="5" t="s">
         <v>13</v>
@@ -5375,19 +5372,19 @@
         <v>149</v>
       </c>
       <c r="B150" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C150" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C150" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D150" s="4">
         <v>11</v>
       </c>
       <c r="E150" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F150" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="F150" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="G150" s="5" t="s">
         <v>13</v>
@@ -5404,19 +5401,19 @@
         <v>150</v>
       </c>
       <c r="B151" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C151" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C151" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D151" s="4">
         <v>12</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G151" s="5" t="s">
         <v>13</v>
@@ -5433,19 +5430,19 @@
         <v>151</v>
       </c>
       <c r="B152" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C152" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C152" s="3" t="s">
-        <v>208</v>
-      </c>
       <c r="D152" s="4">
         <v>13</v>
       </c>
       <c r="E152" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F152" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="F152" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="G152" s="5" t="s">
         <v>13</v>
@@ -5462,19 +5459,19 @@
         <v>152</v>
       </c>
       <c r="B153" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C153" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C153" s="3" t="s">
-        <v>208</v>
-      </c>
       <c r="D153" s="4">
         <v>14</v>
       </c>
       <c r="E153" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="F153" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="F153" s="3" t="s">
-        <v>229</v>
       </c>
       <c r="G153" s="5" t="s">
         <v>13</v>
@@ -5491,10 +5488,10 @@
         <v>153</v>
       </c>
       <c r="B154" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C154" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D154" s="4">
         <v>15</v>
@@ -5520,10 +5517,10 @@
         <v>154</v>
       </c>
       <c r="B155" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C155" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C155" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D155" s="4">
         <v>16</v>
@@ -5549,10 +5546,10 @@
         <v>155</v>
       </c>
       <c r="B156" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C156" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C156" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D156" s="4">
         <v>17</v>
@@ -5578,10 +5575,10 @@
         <v>156</v>
       </c>
       <c r="B157" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C157" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C157" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D157" s="4">
         <v>18</v>
@@ -5607,10 +5604,10 @@
         <v>157</v>
       </c>
       <c r="B158" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C158" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C158" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D158" s="4">
         <v>19</v>
@@ -5636,10 +5633,10 @@
         <v>158</v>
       </c>
       <c r="B159" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C159" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D159" s="4">
         <v>20</v>
@@ -5665,10 +5662,10 @@
         <v>159</v>
       </c>
       <c r="B160" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C160" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D160" s="4">
         <v>1</v>
@@ -5694,19 +5691,19 @@
         <v>160</v>
       </c>
       <c r="B161" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C161" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C161" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D161" s="4">
         <v>2</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G161" s="5" t="s">
         <v>13</v>
@@ -5723,19 +5720,19 @@
         <v>161</v>
       </c>
       <c r="B162" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C162" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D162" s="4">
         <v>3</v>
       </c>
       <c r="E162" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F162" s="3" t="s">
         <v>233</v>
-      </c>
-      <c r="F162" s="3" t="s">
-        <v>234</v>
       </c>
       <c r="G162" s="5" t="s">
         <v>13</v>
@@ -5752,19 +5749,19 @@
         <v>162</v>
       </c>
       <c r="B163" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C163" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D163" s="4">
         <v>4</v>
       </c>
       <c r="E163" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="F163" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="F163" s="3" t="s">
-        <v>236</v>
       </c>
       <c r="G163" s="5" t="s">
         <v>13</v>
@@ -5781,19 +5778,19 @@
         <v>163</v>
       </c>
       <c r="B164" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C164" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D164" s="4">
         <v>5</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G164" s="5" t="s">
         <v>13</v>
@@ -5810,19 +5807,19 @@
         <v>164</v>
       </c>
       <c r="B165" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C165" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C165" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D165" s="4">
         <v>6</v>
       </c>
       <c r="E165" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F165" s="3" t="s">
         <v>238</v>
-      </c>
-      <c r="F165" s="3" t="s">
-        <v>239</v>
       </c>
       <c r="G165" s="5" t="s">
         <v>13</v>
@@ -5839,19 +5836,19 @@
         <v>165</v>
       </c>
       <c r="B166" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C166" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C166" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D166" s="4">
         <v>7</v>
       </c>
       <c r="E166" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F166" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="F166" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="G166" s="5" t="s">
         <v>13</v>
@@ -5868,19 +5865,19 @@
         <v>166</v>
       </c>
       <c r="B167" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C167" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C167" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D167" s="4">
         <v>8</v>
       </c>
       <c r="E167" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F167" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="F167" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="G167" s="5" t="s">
         <v>13</v>
@@ -5889,7 +5886,7 @@
         <v>2000</v>
       </c>
       <c r="I167" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="168" ht="58" customHeight="1">
@@ -5897,19 +5894,19 @@
         <v>167</v>
       </c>
       <c r="B168" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C168" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C168" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D168" s="4">
         <v>9</v>
       </c>
       <c r="E168" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F168" s="3" t="s">
         <v>245</v>
-      </c>
-      <c r="F168" s="3" t="s">
-        <v>246</v>
       </c>
       <c r="G168" s="5" t="s">
         <v>13</v>
@@ -5918,7 +5915,7 @@
         <v>2000</v>
       </c>
       <c r="I168" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="169" ht="58" customHeight="1">
@@ -5926,19 +5923,19 @@
         <v>168</v>
       </c>
       <c r="B169" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C169" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C169" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D169" s="4">
         <v>10</v>
       </c>
       <c r="E169" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="F169" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="F169" s="3" t="s">
-        <v>249</v>
       </c>
       <c r="G169" s="5" t="s">
         <v>13</v>
@@ -5955,19 +5952,19 @@
         <v>169</v>
       </c>
       <c r="B170" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C170" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D170" s="4">
         <v>11</v>
       </c>
       <c r="E170" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="F170" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="F170" s="3" t="s">
-        <v>251</v>
       </c>
       <c r="G170" s="5" t="s">
         <v>13</v>
@@ -5984,19 +5981,19 @@
         <v>170</v>
       </c>
       <c r="B171" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C171" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D171" s="4">
         <v>12</v>
       </c>
       <c r="E171" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="F171" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="F171" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="G171" s="5" t="s">
         <v>13</v>
@@ -6013,19 +6010,19 @@
         <v>171</v>
       </c>
       <c r="B172" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C172" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="C172" s="3" t="s">
-        <v>231</v>
-      </c>
       <c r="D172" s="4">
         <v>13</v>
       </c>
       <c r="E172" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F172" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="F172" s="3" t="s">
-        <v>255</v>
       </c>
       <c r="G172" s="5" t="s">
         <v>13</v>
@@ -6042,10 +6039,10 @@
         <v>172</v>
       </c>
       <c r="B173" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C173" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C173" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D173" s="4">
         <v>14</v>
@@ -6071,19 +6068,19 @@
         <v>173</v>
       </c>
       <c r="B174" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C174" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C174" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D174" s="4">
         <v>15</v>
       </c>
       <c r="E174" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="F174" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="F174" s="3" t="s">
-        <v>257</v>
       </c>
       <c r="G174" s="5" t="s">
         <v>13</v>
@@ -6100,19 +6097,19 @@
         <v>174</v>
       </c>
       <c r="B175" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C175" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C175" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D175" s="4">
         <v>16</v>
       </c>
       <c r="E175" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F175" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="F175" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="G175" s="5" t="s">
         <v>13</v>
@@ -6129,10 +6126,10 @@
         <v>175</v>
       </c>
       <c r="B176" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C176" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C176" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D176" s="4">
         <v>17</v>
@@ -6141,7 +6138,7 @@
         <v>36</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G176" s="5" t="s">
         <v>13</v>
@@ -6158,10 +6155,10 @@
         <v>176</v>
       </c>
       <c r="B177" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C177" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C177" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D177" s="4">
         <v>18</v>
@@ -6187,10 +6184,10 @@
         <v>177</v>
       </c>
       <c r="B178" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C178" s="3" t="s">
         <v>230</v>
-      </c>
-      <c r="C178" s="3" t="s">
-        <v>231</v>
       </c>
       <c r="D178" s="4">
         <v>19</v>

</xml_diff>